<commit_message>
update edit link between pr and po
</commit_message>
<xml_diff>
--- a/public/templates/PO_Form.xlsx
+++ b/public/templates/PO_Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03B600E-CE4F-474F-B98A-C563C0673552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A95053-1253-4F95-A046-EE522669DFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -897,41 +897,6 @@
     <xf numFmtId="43" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -987,6 +952,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1515,8 +1515,8 @@
   </sheetPr>
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="208" zoomScaleNormal="100" zoomScaleSheetLayoutView="208" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="208" zoomScaleNormal="100" zoomScaleSheetLayoutView="208" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1532,7 +1532,7 @@
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18">
+    <row r="1" spans="2:10" ht="15.75">
       <c r="B1" s="5"/>
       <c r="C1" s="54" t="s">
         <v>28</v>
@@ -1579,16 +1579,16 @@
       <c r="D4" s="5"/>
       <c r="E4" s="21"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:10" s="44" customFormat="1" ht="18.75">
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
+    <row r="5" spans="2:10" s="44" customFormat="1" ht="17.25">
+      <c r="B5" s="105"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
       <c r="F5" s="45" t="s">
         <v>16</v>
       </c>
@@ -1611,8 +1611,8 @@
       <c r="B7" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
       <c r="F7" s="45" t="s">
         <v>1</v>
       </c>
@@ -1643,10 +1643,10 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:10" s="44" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="85"/>
+      <c r="C10" s="106"/>
       <c r="D10" s="2"/>
       <c r="E10" s="67"/>
       <c r="F10" s="2"/>
@@ -1654,19 +1654,19 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:10" ht="21">
-      <c r="B11" s="77" t="s">
+    <row r="11" spans="2:10" ht="18.75">
+      <c r="B11" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="78"/>
-      <c r="D11" s="80" t="s">
+      <c r="C11" s="99"/>
+      <c r="D11" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="80" t="s">
+      <c r="E11" s="99"/>
+      <c r="F11" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="78"/>
+      <c r="G11" s="99"/>
       <c r="H11" s="28" t="s">
         <v>21</v>
       </c>
@@ -1674,12 +1674,12 @@
       <c r="J11" s="28"/>
     </row>
     <row r="12" spans="2:10" ht="13.5" customHeight="1">
-      <c r="B12" s="79"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="78"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="99"/>
       <c r="H12" s="43"/>
       <c r="I12" s="1"/>
     </row>
@@ -1694,20 +1694,20 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="97"/>
-      <c r="E14" s="92" t="s">
+      <c r="D14" s="84"/>
+      <c r="E14" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="92" t="s">
+      <c r="F14" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="94" t="s">
+      <c r="G14" s="81" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="31" t="s">
@@ -1716,12 +1716,12 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1">
-      <c r="B15" s="91"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="95"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="82"/>
       <c r="H15" s="52" t="s">
         <v>17</v>
       </c>
@@ -1768,8 +1768,8 @@
     </row>
     <row r="19" spans="2:9" ht="21.75" customHeight="1">
       <c r="B19" s="48"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="75"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="61"/>
       <c r="F19" s="50"/>
       <c r="G19" s="59"/>
@@ -1820,8 +1820,8 @@
     </row>
     <row r="23" spans="2:9" ht="21.75" customHeight="1">
       <c r="B23" s="48"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="75"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="61"/>
       <c r="F23" s="50"/>
       <c r="G23" s="59"/>
@@ -1833,8 +1833,8 @@
     </row>
     <row r="24" spans="2:9" ht="21.75" customHeight="1">
       <c r="B24" s="48"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="75"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="61"/>
       <c r="F24" s="50"/>
       <c r="G24" s="59"/>
@@ -1885,8 +1885,8 @@
     </row>
     <row r="28" spans="2:9" ht="21.75" customHeight="1">
       <c r="B28" s="48"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="51"/>
       <c r="F28" s="50"/>
       <c r="G28" s="63"/>
@@ -1898,8 +1898,8 @@
     </row>
     <row r="29" spans="2:9" ht="21.75" customHeight="1">
       <c r="B29" s="48"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="96"/>
       <c r="E29" s="51"/>
       <c r="F29" s="50"/>
       <c r="G29" s="63"/>
@@ -2011,13 +2011,13 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1">
-      <c r="B37" s="100" t="str">
+      <c r="B37" s="87" t="str">
         <f>BAHTTEXT(H37)</f>
         <v>ศูนย์บาทถ้วน</v>
       </c>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="102"/>
+      <c r="C37" s="88"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="89"/>
       <c r="F37" s="11" t="s">
         <v>13</v>
       </c>
@@ -2039,54 +2039,54 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="103"/>
+      <c r="C39" s="90"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="12"/>
-      <c r="G39" s="103"/>
-      <c r="H39" s="104"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="91"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="2:10" ht="19.5" customHeight="1">
-      <c r="B40" s="107"/>
-      <c r="C40" s="103"/>
+      <c r="B40" s="94"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="103"/>
-      <c r="H40" s="104"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="91"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B41" s="105" t="s">
+      <c r="B41" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="106"/>
+      <c r="C41" s="93"/>
       <c r="D41" s="24"/>
       <c r="E41" s="27" t="s">
         <v>20</v>
       </c>
       <c r="F41" s="27"/>
-      <c r="G41" s="88"/>
-      <c r="H41" s="89"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="76"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="21">
+    <row r="42" spans="2:10" ht="18.75">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="12"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="87"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:10" ht="21">
+    <row r="43" spans="2:10" ht="18.75">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2096,7 +2096,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:10" ht="21">
+    <row r="44" spans="2:10" ht="18.75">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2106,7 +2106,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:10" ht="21">
+    <row r="45" spans="2:10" ht="18.75">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2116,7 +2116,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:10" ht="21">
+    <row r="46" spans="2:10" ht="18.75">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2126,7 +2126,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:10" ht="21">
+    <row r="47" spans="2:10" ht="18.75">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2136,7 +2136,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="2:10" ht="21">
+    <row r="48" spans="2:10" ht="18.75">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2146,7 +2146,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" ht="21">
+    <row r="49" spans="2:9" ht="18.75">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2156,7 +2156,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" ht="21">
+    <row r="50" spans="2:9" ht="18.75">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2166,7 +2166,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="2:9" ht="21">
+    <row r="51" spans="2:9" ht="18.75">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2176,7 +2176,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" ht="21">
+    <row r="52" spans="2:9" ht="18.75">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2186,7 +2186,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:9" ht="21">
+    <row r="53" spans="2:9" ht="18.75">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2196,7 +2196,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="2:9" ht="21">
+    <row r="54" spans="2:9" ht="18.75">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2206,7 +2206,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="2:9" ht="21">
+    <row r="55" spans="2:9" ht="18.75">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2216,7 +2216,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="2:9" ht="21">
+    <row r="56" spans="2:9" ht="18.75">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2226,7 +2226,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="2:9" ht="21">
+    <row r="57" spans="2:9" ht="18.75">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2236,7 +2236,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="2:9" ht="21">
+    <row r="58" spans="2:9" ht="18.75">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2246,7 +2246,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="2:9" ht="21">
+    <row r="59" spans="2:9" ht="18.75">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2256,7 +2256,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="2:9" ht="21">
+    <row r="60" spans="2:9" ht="18.75">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2266,7 +2266,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="2:9" ht="21">
+    <row r="61" spans="2:9" ht="18.75">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2276,7 +2276,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="2:9" ht="21">
+    <row r="62" spans="2:9" ht="18.75">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2286,7 +2286,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="2:9" ht="21">
+    <row r="63" spans="2:9" ht="18.75">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2296,7 +2296,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="2:9" ht="21">
+    <row r="64" spans="2:9" ht="18.75">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2306,7 +2306,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:9" ht="21">
+    <row r="65" spans="2:9" ht="18.75">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2316,7 +2316,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="2:9" ht="21">
+    <row r="66" spans="2:9" ht="18.75">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2326,7 +2326,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="2:9" ht="21">
+    <row r="67" spans="2:9" ht="18.75">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2336,7 +2336,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="2:9" ht="21">
+    <row r="68" spans="2:9" ht="18.75">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2346,7 +2346,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="2:9" ht="21">
+    <row r="69" spans="2:9" ht="18.75">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2356,7 +2356,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" ht="21">
+    <row r="70" spans="2:9" ht="18.75">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2366,7 +2366,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" ht="21">
+    <row r="71" spans="2:9" ht="18.75">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2376,7 +2376,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:9" ht="21">
+    <row r="72" spans="2:9" ht="18.75">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2386,7 +2386,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="2:9" ht="21">
+    <row r="73" spans="2:9" ht="18.75">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2396,7 +2396,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="2:9" ht="21">
+    <row r="74" spans="2:9" ht="18.75">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2406,7 +2406,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="2:9" ht="21">
+    <row r="75" spans="2:9" ht="18.75">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2416,7 +2416,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:9" ht="21">
+    <row r="76" spans="2:9" ht="18.75">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2426,7 +2426,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="2:9" ht="21">
+    <row r="77" spans="2:9" ht="18.75">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2436,7 +2436,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="2:9" ht="21">
+    <row r="78" spans="2:9" ht="18.75">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2446,7 +2446,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="2:9" ht="21">
+    <row r="79" spans="2:9" ht="18.75">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2456,7 +2456,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="2:9" ht="21">
+    <row r="80" spans="2:9" ht="18.75">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2466,7 +2466,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="2:9" ht="21">
+    <row r="81" spans="2:9" ht="18.75">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2476,7 +2476,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="2:9" ht="21">
+    <row r="82" spans="2:9" ht="18.75">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2486,7 +2486,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="2:9" ht="21">
+    <row r="83" spans="2:9" ht="18.75">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2496,7 +2496,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="2:9" ht="21">
+    <row r="84" spans="2:9" ht="18.75">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2506,7 +2506,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="2:9" ht="21">
+    <row r="85" spans="2:9" ht="18.75">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2517,6 +2517,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B14:B15"/>
@@ -2533,23 +2545,11 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="89" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
Add export Pr and Po List
</commit_message>
<xml_diff>
--- a/public/templates/PO_Form.xlsx
+++ b/public/templates/PO_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C225D0-3915-4A5A-8F0F-8D3995CBFFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E291DE33-7341-4B81-809F-AB67369B1E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,7 +147,7 @@
     <numFmt numFmtId="167" formatCode="##"/>
     <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +315,11 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Angsana New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Angsana New"/>
       <family val="1"/>
     </font>
@@ -778,9 +783,6 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -852,85 +854,6 @@
     </xf>
     <xf numFmtId="43" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -938,23 +861,105 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1482,53 +1487,53 @@
   <dimension ref="B1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="93" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="93" customWidth="1"/>
-    <col min="3" max="3" width="33" style="93" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="93" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="103" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="93" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="104" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="93" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="93"/>
-    <col min="10" max="10" width="9.42578125" style="93" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="93"/>
+    <col min="1" max="1" width="2.140625" style="65" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="33" style="65" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="65" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="69" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="65" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="70" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="65" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="65"/>
+    <col min="10" max="10" width="9.42578125" style="65" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="65"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:10" ht="15.75">
       <c r="B1" s="5"/>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="5"/>
-      <c r="E1" s="47"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="5"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="47"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:10" ht="13.5" customHeight="1">
       <c r="B3" s="5"/>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="5"/>
@@ -1539,82 +1544,82 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:10" ht="17.25" customHeight="1">
       <c r="B4" s="5"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="17"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="39" t="s">
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="16.5">
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="94"/>
-    </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="62"/>
-      <c r="D6" s="95"/>
-      <c r="F6" s="39" t="s">
+      <c r="G5" s="66"/>
+    </row>
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B6" s="61"/>
+      <c r="D6" s="67"/>
+      <c r="F6" s="38" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="59" t="s">
+    <row r="7" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B7" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="F7" s="39" t="s">
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="F7" s="38" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="F8" s="39"/>
+      <c r="C8" s="64"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="39" t="s">
+    <row r="9" spans="2:10" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="B9" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="60"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="73" t="s">
+    <row r="10" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B10" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="102"/>
+      <c r="E10" s="60"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="21" x14ac:dyDescent="0.45">
-      <c r="B11" s="68" t="s">
+    <row r="11" spans="2:10" ht="18.75">
+      <c r="B11" s="95" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="96"/>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="98" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="96"/>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="98" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="96"/>
@@ -1624,17 +1629,17 @@
       <c r="I11" s="1"/>
       <c r="J11" s="24"/>
     </row>
-    <row r="12" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="69"/>
+    <row r="12" spans="2:10" ht="13.5" customHeight="1">
+      <c r="B12" s="97"/>
       <c r="C12" s="96"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="72"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="101"/>
       <c r="G12" s="96"/>
-      <c r="H12" s="38"/>
+      <c r="H12" s="104"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:10" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:10" ht="3" customHeight="1" thickBot="1">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1644,21 +1649,21 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="78" t="s">
+    <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B14" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="83" t="s">
+      <c r="C14" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="79" t="s">
+      <c r="D14" s="81"/>
+      <c r="E14" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="79" t="s">
+      <c r="F14" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="81" t="s">
+      <c r="G14" s="78" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="27" t="s">
@@ -1666,242 +1671,242 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="99"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="46" t="s">
+    <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1">
+      <c r="B15" s="75"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="45" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="49"/>
+    <row r="16" spans="2:10" ht="21.75" customHeight="1">
+      <c r="B16" s="48"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="63">
+      <c r="D16" s="51"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="62">
         <f>F16*G16</f>
         <v>0</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="54"/>
+    <row r="17" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B17" s="53"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="64">
+      <c r="D17" s="42"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="63">
         <f>F17*G17</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="42"/>
+    <row r="18" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B18" s="41"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="64">
+      <c r="D18" s="57"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="63">
         <f t="shared" ref="H18:H32" si="0">F18*G18</f>
         <v>0</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="42"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="64">
+    <row r="19" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B19" s="41"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="54"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="64">
+    <row r="20" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B20" s="53"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="42"/>
+    <row r="21" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B21" s="41"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="64">
+      <c r="D21" s="51"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="54"/>
+    <row r="22" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B22" s="53"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="64">
+      <c r="D22" s="42"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="42"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="64">
+    <row r="23" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B23" s="41"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="42"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="64">
+    <row r="24" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B24" s="41"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="42"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="64">
+    <row r="25" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B25" s="41"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="42"/>
+    <row r="26" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B26" s="41"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="64">
+      <c r="D26" s="51"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="42"/>
+    <row r="27" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B27" s="41"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="64">
+      <c r="D27" s="42"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="42"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="64">
+    <row r="28" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B28" s="41"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="42"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="64">
+    <row r="29" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B29" s="41"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="42"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="64">
+    <row r="30" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B30" s="41"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="42"/>
+    <row r="31" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B31" s="41"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="64">
+      <c r="D31" s="42"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="2:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:9" ht="21.75" customHeight="1" thickBot="1">
       <c r="B32" s="25"/>
       <c r="C32" s="29"/>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="25"/>
       <c r="G32" s="28"/>
-      <c r="H32" s="64">
+      <c r="H32" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:10" ht="24.75" customHeight="1">
       <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
@@ -1918,7 +1923,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:10" ht="22.5" customHeight="1">
       <c r="B34" s="4"/>
       <c r="C34" s="12"/>
       <c r="D34" s="1"/>
@@ -1927,12 +1932,12 @@
         <v>10</v>
       </c>
       <c r="G34" s="31"/>
-      <c r="H34" s="51"/>
+      <c r="H34" s="50"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:10" ht="22.5" customHeight="1">
       <c r="B35" s="4"/>
-      <c r="C35" s="40"/>
+      <c r="C35" s="39"/>
       <c r="D35" s="1"/>
       <c r="E35" s="12"/>
       <c r="F35" s="9" t="s">
@@ -1944,9 +1949,9 @@
         <v>0</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="102"/>
-    </row>
-    <row r="36" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J35" s="68"/>
+    </row>
+    <row r="36" spans="2:10" ht="22.5" customHeight="1" thickBot="1">
       <c r="B36" s="4"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1961,7 +1966,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1">
       <c r="B37" s="84" t="str">
         <f>BAHTTEXT(H37)</f>
         <v>ศูนย์บาทถ้วน</v>
@@ -1979,7 +1984,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:10" ht="27.75" customHeight="1">
       <c r="B38" s="3"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
@@ -1989,7 +1994,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:10" ht="34.5" customHeight="1">
       <c r="B39" s="91" t="s">
         <v>27</v>
       </c>
@@ -2003,7 +2008,7 @@
       <c r="H39" s="88"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:10" ht="19.5" customHeight="1">
       <c r="B40" s="91"/>
       <c r="C40" s="87"/>
       <c r="D40" s="12"/>
@@ -2013,7 +2018,7 @@
       <c r="H40" s="88"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1">
       <c r="B41" s="89" t="s">
         <v>26</v>
       </c>
@@ -2023,21 +2028,21 @@
         <v>20</v>
       </c>
       <c r="F41" s="23"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="77"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="73"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:10" ht="18.75">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="12"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:10" ht="18.75">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2047,7 +2052,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" ht="18.75">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2057,7 +2062,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:10" ht="18.75">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2067,7 +2072,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:10" ht="18.75">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2077,7 +2082,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:10" ht="18.75">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2087,7 +2092,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="2:10" ht="21" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:10" ht="18.75">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2097,7 +2102,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:9" ht="18.75">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2107,7 +2112,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:9" ht="18.75">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2117,7 +2122,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:9" ht="18.75">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2127,7 +2132,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:9" ht="18.75">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2137,7 +2142,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:9" ht="18.75">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2147,7 +2152,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:9" ht="18.75">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2157,7 +2162,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:9" ht="18.75">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2167,7 +2172,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:9" ht="18.75">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2177,7 +2182,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:9" ht="18.75">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2187,7 +2192,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:9" ht="18.75">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2197,7 +2202,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:9" ht="18.75">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2207,7 +2212,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:9" ht="18.75">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2217,7 +2222,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:9" ht="18.75">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2227,7 +2232,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:9" ht="18.75">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2237,7 +2242,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:9" ht="18.75">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2247,7 +2252,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:9" ht="18.75">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2257,7 +2262,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:9" ht="18.75">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2267,7 +2272,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:9" ht="18.75">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2277,7 +2282,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:9" ht="18.75">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2287,7 +2292,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:9" ht="18.75">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2297,7 +2302,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:9" ht="18.75">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2307,7 +2312,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:9" ht="18.75">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2317,7 +2322,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:9" ht="18.75">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2327,7 +2332,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:9" ht="18.75">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2337,7 +2342,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:9" ht="18.75">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2347,7 +2352,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:9" ht="18.75">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2357,7 +2362,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:9" ht="18.75">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2367,7 +2372,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:9" ht="18.75">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2377,7 +2382,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:9" ht="18.75">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2387,7 +2392,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:9" ht="18.75">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2397,7 +2402,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:9" ht="18.75">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2407,7 +2412,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:9" ht="18.75">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2417,7 +2422,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:9" ht="18.75">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2427,7 +2432,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:9" ht="18.75">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2437,7 +2442,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:9" ht="18.75">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2447,7 +2452,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:9" ht="18.75">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2457,7 +2462,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="2:9" ht="21" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:9" ht="18.75">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2468,6 +2473,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B14:B15"/>
@@ -2484,23 +2501,11 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="89" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
fixing max 17 item
</commit_message>
<xml_diff>
--- a/public/templates/PO_Form.xlsx
+++ b/public/templates/PO_Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C9F7AA-83B6-403C-AD11-254161D9FD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2534A192-A8CD-4C6E-9E9C-458D5D68F012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,15 +139,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;฿&quot;\t#,##0_);[Red]\(&quot;฿&quot;\t#,##0\)"/>
     <numFmt numFmtId="166" formatCode="#,###.#"/>
     <numFmt numFmtId="167" formatCode="##"/>
     <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.00;\-0.00;;@"/>
+    <numFmt numFmtId="170" formatCode="0;\-0;;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,7 +716,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,7 +765,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -796,9 +797,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -823,9 +821,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -833,9 +828,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -869,6 +861,12 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -959,6 +957,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="30">
@@ -1486,54 +1496,54 @@
   </sheetPr>
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="65" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="65" customWidth="1"/>
-    <col min="3" max="3" width="33" style="65" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="65" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="69" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="65" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="70" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="65" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="65"/>
-    <col min="10" max="10" width="9.42578125" style="65" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="65"/>
+    <col min="1" max="1" width="2.140625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="33" style="61" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="61" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="66" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="61" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="61"/>
+    <col min="10" max="10" width="9.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75">
       <c r="B1" s="5"/>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="5"/>
-      <c r="E1" s="46"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="5"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="45" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="46"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="13.5" customHeight="1">
       <c r="B3" s="5"/>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="5"/>
@@ -1544,102 +1554,102 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="17.25" customHeight="1">
       <c r="B4" s="5"/>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="45" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="17"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="38" t="s">
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="16.5">
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="66"/>
-    </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="61"/>
-      <c r="D6" s="67"/>
-      <c r="F6" s="38" t="s">
+      <c r="G5" s="62"/>
+    </row>
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B6" s="57"/>
+      <c r="D6" s="63"/>
+      <c r="F6" s="37" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="58" t="s">
+    <row r="7" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B7" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="F7" s="38" t="s">
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="F7" s="37" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="19"/>
     </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="F8" s="38"/>
+      <c r="C8" s="60"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+    <row r="9" spans="2:10" s="2" customFormat="1" ht="18" customHeight="1">
+      <c r="B9" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="60"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="103" t="s">
+    <row r="10" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B10" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="103"/>
-      <c r="E10" s="60"/>
+      <c r="C10" s="101"/>
+      <c r="E10" s="56"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="96" t="s">
+    <row r="11" spans="2:10" ht="18.75">
+      <c r="B11" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="97"/>
-      <c r="D11" s="99" t="s">
+      <c r="C11" s="95"/>
+      <c r="D11" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="97"/>
-      <c r="F11" s="99" t="s">
+      <c r="E11" s="95"/>
+      <c r="F11" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="97"/>
+      <c r="G11" s="95"/>
       <c r="H11" s="24" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="24"/>
     </row>
-    <row r="12" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="98"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="71"/>
+    <row r="12" spans="2:10" ht="13.5" customHeight="1">
+      <c r="B12" s="96"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:10" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="3" customHeight="1" thickBot="1">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1649,21 +1659,21 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="75" t="s">
+    <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B14" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="77" t="s">
+      <c r="D14" s="80"/>
+      <c r="E14" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="79" t="s">
+      <c r="G14" s="77" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="27" t="s">
@@ -1671,242 +1681,242 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="76"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="45" t="s">
+    <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1">
+      <c r="B15" s="74"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="43" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="48"/>
+    <row r="16" spans="2:10" ht="21.75" customHeight="1">
+      <c r="B16" s="46"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="62">
+      <c r="D16" s="49"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="58">
         <f>F16*G16</f>
         <v>0</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="53"/>
+    <row r="17" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B17" s="50"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="63">
+      <c r="D17" s="41"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="59">
         <f>F17*G17</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
+    <row r="18" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B18" s="40"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="63">
+      <c r="D18" s="53"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="59">
         <f t="shared" ref="H18:H32" si="0">F18*G18</f>
         <v>0</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="63">
+    <row r="19" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B19" s="40"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="53"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="63">
+    <row r="20" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B20" s="50"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="41"/>
+    <row r="21" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B21" s="40"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="63">
+      <c r="D21" s="49"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="53"/>
+    <row r="22" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B22" s="50"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="63">
+      <c r="D22" s="41"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="41"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="63">
+    <row r="23" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B23" s="40"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="41"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="63">
+    <row r="24" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B24" s="40"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="41"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="63">
+    <row r="25" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B25" s="40"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+    <row r="26" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B26" s="40"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="63">
+      <c r="D26" s="49"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="41"/>
+    <row r="27" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B27" s="40"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="63">
+      <c r="D27" s="41"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="41"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="63">
+    <row r="28" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B28" s="40"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="41"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="63">
+    <row r="29" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B29" s="40"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="92"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="41"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="63">
+    <row r="30" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B30" s="40"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="41"/>
+    <row r="31" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B31" s="40"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="63">
+      <c r="D31" s="41"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="2:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" ht="21.75" customHeight="1" thickBot="1">
       <c r="B32" s="25"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="40" t="s">
+      <c r="C32" s="28"/>
+      <c r="D32" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="26"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="63">
+      <c r="F32" s="105"/>
+      <c r="G32" s="106"/>
+      <c r="H32" s="59">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" ht="24.75" customHeight="1">
       <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
@@ -1916,14 +1926,14 @@
       <c r="F33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="30"/>
-      <c r="H33" s="34">
+      <c r="G33" s="29"/>
+      <c r="H33" s="33">
         <f>SUM(H16:H32)</f>
         <v>0</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="22.5" customHeight="1">
       <c r="B34" s="4"/>
       <c r="C34" s="12"/>
       <c r="D34" s="1"/>
@@ -1931,27 +1941,27 @@
       <c r="F34" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="50"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="48"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="22.5" customHeight="1">
       <c r="B35" s="4"/>
-      <c r="C35" s="39"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="1"/>
       <c r="E35" s="12"/>
       <c r="F35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="31"/>
-      <c r="H35" s="35">
+      <c r="G35" s="30"/>
+      <c r="H35" s="34">
         <f>H33-H34</f>
         <v>0</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="68"/>
-    </row>
-    <row r="36" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="64"/>
+    </row>
+    <row r="36" spans="2:10" ht="22.5" customHeight="1" thickBot="1">
       <c r="B36" s="4"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1959,32 +1969,32 @@
       <c r="F36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="32"/>
-      <c r="H36" s="36">
+      <c r="G36" s="31"/>
+      <c r="H36" s="35">
         <f>H35*7%</f>
         <v>0</v>
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="85" t="str">
+    <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1">
+      <c r="B37" s="83" t="str">
         <f>BAHTTEXT(H37)</f>
         <v>ศูนย์บาทถ้วน</v>
       </c>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="87"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="85"/>
       <c r="F37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="33"/>
-      <c r="H37" s="37">
+      <c r="G37" s="32"/>
+      <c r="H37" s="36">
         <f>H35+H36</f>
         <v>0</v>
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" ht="27.75" customHeight="1">
       <c r="B38" s="3"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
@@ -1994,55 +2004,55 @@
       <c r="H38" s="6"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="92" t="s">
+    <row r="39" spans="2:10" ht="34.5" customHeight="1">
+      <c r="B39" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="88"/>
+      <c r="C39" s="86"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="12"/>
-      <c r="G39" s="88"/>
-      <c r="H39" s="89"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="87"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="92"/>
-      <c r="C40" s="88"/>
+    <row r="40" spans="2:10" ht="19.5" customHeight="1">
+      <c r="B40" s="90"/>
+      <c r="C40" s="86"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="88"/>
-      <c r="H40" s="89"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="87"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="90" t="s">
+    <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B41" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="91"/>
+      <c r="C41" s="89"/>
       <c r="D41" s="20"/>
       <c r="E41" s="23" t="s">
         <v>20</v>
       </c>
       <c r="F41" s="23"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="74"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="72"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" ht="18.75">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="12"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="72"/>
-      <c r="H42" s="72"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" ht="18.75">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2052,7 +2062,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" ht="18.75">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2062,7 +2072,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:10" ht="18.75">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2072,7 +2082,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" ht="18.75">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2082,7 +2092,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:10" ht="18.75">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2092,7 +2102,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" ht="18.75">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2102,7 +2112,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" ht="18.75">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2112,7 +2122,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" ht="18.75">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2122,7 +2132,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" ht="18.75">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2132,7 +2142,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" ht="18.75">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2142,7 +2152,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" ht="18.75">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2152,7 +2162,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" ht="18.75">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2162,7 +2172,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" ht="18.75">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2172,7 +2182,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" ht="18.75">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2182,7 +2192,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" ht="18.75">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2192,7 +2202,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" ht="18.75">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2202,7 +2212,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" ht="18.75">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2212,7 +2222,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" ht="18.75">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2222,7 +2232,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" ht="18.75">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2232,7 +2242,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" ht="18.75">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2242,7 +2252,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" ht="18.75">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2252,7 +2262,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" ht="18.75">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2262,7 +2272,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" ht="18.75">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2272,7 +2282,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" ht="18.75">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2282,7 +2292,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" ht="18.75">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2292,7 +2302,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" ht="18.75">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2302,7 +2312,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" ht="18.75">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2312,7 +2322,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" ht="18.75">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2322,7 +2332,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" ht="18.75">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2332,7 +2342,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" ht="18.75">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2342,7 +2352,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" ht="18.75">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2352,7 +2362,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" ht="18.75">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2362,7 +2372,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" ht="18.75">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2372,7 +2382,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" ht="18.75">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2382,7 +2392,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" ht="18.75">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2392,7 +2402,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" ht="18.75">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2402,7 +2412,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" ht="18.75">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2412,7 +2422,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" ht="18.75">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2422,7 +2432,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" ht="18.75">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2432,7 +2442,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:9" ht="18.75">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2442,7 +2452,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:9" ht="18.75">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2452,7 +2462,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" ht="18.75">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2462,7 +2472,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:9" ht="18.75">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>

</xml_diff>

<commit_message>
Change PR PO XLSX
</commit_message>
<xml_diff>
--- a/public/templates/PO_Form.xlsx
+++ b/public/templates/PO_Form.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8C5DFD-9E0D-41B8-A46D-C639792F4A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0141A673-3A82-4676-89B6-31318F7878B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Page 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$H$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$B$1:$H$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="273">
   <si>
     <t>PO  NO.  :</t>
   </si>
@@ -111,9 +112,6 @@
     <t xml:space="preserve">Website : www.mot.co.th                                                                                                               </t>
   </si>
   <si>
-    <t>หน้า 1 ของ 1 หน้า</t>
-  </si>
-  <si>
     <t>PURCHASING</t>
   </si>
   <si>
@@ -132,7 +130,730 @@
     <t xml:space="preserve">TEX ID  </t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
+    <t>Power Bar Toshino ET-9165M (5M) White</t>
+  </si>
+  <si>
+    <t>670001-IT-MOT</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>รายการ</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>tkt</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>IT-67-04-002</t>
+  </si>
+  <si>
+    <t>IT-67-04-001</t>
+  </si>
+  <si>
+    <t>670002-IT-MOT</t>
+  </si>
+  <si>
+    <t>Dept.</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.Suwat </t>
+  </si>
+  <si>
+    <t>K.natthapong</t>
+  </si>
+  <si>
+    <t>IT-67-04-003</t>
+  </si>
+  <si>
+    <t>IT-67-04-004</t>
+  </si>
+  <si>
+    <t>670003-IT-MOT</t>
+  </si>
+  <si>
+    <t>670004-IT-MOT</t>
+  </si>
+  <si>
+    <t>Adapter notebook + wireless mouse</t>
+  </si>
+  <si>
+    <t>Ram 8 GB x2 For Notebook</t>
+  </si>
+  <si>
+    <t>K.Phonglit</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">บริษัท เจเจเน็ตเวิร์ค 2022 </t>
+  </si>
+  <si>
+    <t>FotiAnalyzer 200D (มือสอง)</t>
+  </si>
+  <si>
+    <t>IT-67-04-005</t>
+  </si>
+  <si>
+    <t>670005-IT-MOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FotiGate 61E Storage SSD 128GB USED, MA Expired </t>
+  </si>
+  <si>
+    <t>MNET CORPORATION CO., LTD. (Head Office)</t>
+  </si>
+  <si>
+    <t>IT-67-04-006</t>
+  </si>
+  <si>
+    <t>670006-IT-MOT</t>
+  </si>
+  <si>
+    <t>Monitor : Samsung 24,Flat</t>
+  </si>
+  <si>
+    <t>T.K.T PROFESSIONAL CO.,LTD.</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Natthaphong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surasak </t>
+  </si>
+  <si>
+    <t>IT-67-04-007</t>
+  </si>
+  <si>
+    <t>Renew Licesce Office365</t>
+  </si>
+  <si>
+    <t>670007-IT-MOT</t>
+  </si>
+  <si>
+    <t>IT-67-04-008</t>
+  </si>
+  <si>
+    <t>670008-IT-MOT</t>
+  </si>
+  <si>
+    <t>Furinbox เก้าอี้สำนักงาน รุ่นดาร์บี้ - สีดำ</t>
+  </si>
+  <si>
+    <t>บริษัท อินเด็กซ์ ลิฟวิ่งมอลล์ จำกัด (มหาชน)</t>
+  </si>
+  <si>
+    <t>IT-67-04-009</t>
+  </si>
+  <si>
+    <t>670009-IT-MOT</t>
+  </si>
+  <si>
+    <t>K.Korawit</t>
+  </si>
+  <si>
+    <t>Transcend 8GB DDR3‐1600 for PC</t>
+  </si>
+  <si>
+    <t>IT-67-04-0010</t>
+  </si>
+  <si>
+    <t>6700010-IT-MOT</t>
+  </si>
+  <si>
+    <t>ESET PROTECT Entry ‐ 1YN</t>
+  </si>
+  <si>
+    <t>IT-67-04-0011</t>
+  </si>
+  <si>
+    <t>6700011-IT-MOT</t>
+  </si>
+  <si>
+    <t>หมึก</t>
+  </si>
+  <si>
+    <t>IT-67-04-0012</t>
+  </si>
+  <si>
+    <t>6700012-IT-MOT</t>
+  </si>
+  <si>
+    <t>Windown Server 2022 Standard -16 Core License Pack_Commaercial</t>
+  </si>
+  <si>
+    <t>IT-67-04-0013</t>
+  </si>
+  <si>
+    <t>6700013-IT-MOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Pro 11 64Bit Eng Intl 1pk DSP OEI DVD Office Home and </t>
+  </si>
+  <si>
+    <t>Business 2021 English APAC EM Medialess FPP</t>
+  </si>
+  <si>
+    <t>IT-67-04-0014</t>
+  </si>
+  <si>
+    <t>6700014-IT-MOT</t>
+  </si>
+  <si>
+    <t>Cisco Catalyst 1300 24 port (Part# : C1300‐24T‐4G)</t>
+  </si>
+  <si>
+    <t>IT-67-04-0015</t>
+  </si>
+  <si>
+    <t>6700015-IT-MOT</t>
+  </si>
+  <si>
+    <t>IT-67-04-0016</t>
+  </si>
+  <si>
+    <t>6700016-IT-MOT</t>
+  </si>
+  <si>
+    <t>Fiber Optic Cable 12 Core Singlel Mode</t>
+  </si>
+  <si>
+    <t>VanDeeLertKit Co.,Ltd.(Head Office)</t>
+  </si>
+  <si>
+    <t>IT-67-04-0017</t>
+  </si>
+  <si>
+    <t>6700017-IT-MOT</t>
+  </si>
+  <si>
+    <t>APC EASY UPS BV 500VA, AVR, Universal Outlet, 230V</t>
+  </si>
+  <si>
+    <t>IT-67-04-0018</t>
+  </si>
+  <si>
+    <t>APC Easy UPS, 650VA, Floor/Wall Mount, 230V, 4x Universal outlets, AVR</t>
+  </si>
+  <si>
+    <t>IT-67-04-0019</t>
+  </si>
+  <si>
+    <t>6700019-IT-MOT</t>
+  </si>
+  <si>
+    <t>Setup &amp; Commissioning Program Biotime (Remote Online )</t>
+  </si>
+  <si>
+    <t>6700018-IT-MOT</t>
+  </si>
+  <si>
+    <t>AttitudeCom Total Solution and Service Co.,Ltd</t>
+  </si>
+  <si>
+    <t>IT-67-04-0020</t>
+  </si>
+  <si>
+    <t>6700020-IT-MOT</t>
+  </si>
+  <si>
+    <t>IT-67-04-0021</t>
+  </si>
+  <si>
+    <t>6700021-IT-MOT</t>
+  </si>
+  <si>
+    <t>DELL Latitude 3440 (Part# : SNS3440020)</t>
+  </si>
+  <si>
+    <t>ESD-Office Home and Business 2021 All Lng APAC EM PK Lic Online</t>
+  </si>
+  <si>
+    <t>Lenovo V15 G4 i5-13420H/16GB/512GB SSD/15.6ʺ</t>
+  </si>
+  <si>
+    <t>IT-67-04-0022</t>
+  </si>
+  <si>
+    <t>6700022-IT-MOT</t>
+  </si>
+  <si>
+    <t>Kingston XS1000 1TB SSD | Pocket-Sized |</t>
+  </si>
+  <si>
+    <t>IT-67-04-0023</t>
+  </si>
+  <si>
+    <t>6700023-IT-MOT</t>
+  </si>
+  <si>
+    <t>Notebook “Lenovo” V15 G4 i5-13420H/16GB/512GB SSD/15.6ʺ/DOS</t>
+  </si>
+  <si>
+    <t>Office Home and Business 2024 All Lng APAC EM Retail Online ESD</t>
+  </si>
+  <si>
+    <t>IT-67-04-0024</t>
+  </si>
+  <si>
+    <t>6700024-IT-MOT</t>
+  </si>
+  <si>
+    <t>TP-LINK AC1200 Wireless Dual Band 4G LTE Router with 4 x 10/100</t>
+  </si>
+  <si>
+    <t>Office-TECH</t>
+  </si>
+  <si>
+    <t>IT-67-04-0025</t>
+  </si>
+  <si>
+    <t>6700025-IT-MOT</t>
+  </si>
+  <si>
+    <t>Licence Window 11pro</t>
+  </si>
+  <si>
+    <t>P'Susee</t>
+  </si>
+  <si>
+    <t>IT-67-04-0026</t>
+  </si>
+  <si>
+    <t>6700026-IT-MOT</t>
+  </si>
+  <si>
+    <t>Battery Asus VivoBook D413IA-EB249TS Black (A)</t>
+  </si>
+  <si>
+    <t>P'Tui</t>
+  </si>
+  <si>
+    <t>ฝ่ายบริหาร</t>
+  </si>
+  <si>
+    <t>IT-67-04-0027</t>
+  </si>
+  <si>
+    <t>6700027-IT-MOT</t>
+  </si>
+  <si>
+    <t>P'Path</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Transcend 8GB DDR3L-1600 FOR PC PN : TS1GLK64W6H</t>
+  </si>
+  <si>
+    <t>IT-67-04-0028</t>
+  </si>
+  <si>
+    <t>6700028-IT-MOT</t>
+  </si>
+  <si>
+    <t>IT-67-04-0029</t>
+  </si>
+  <si>
+    <t>6700029-IT-MOT</t>
+  </si>
+  <si>
+    <t>IT-6800010</t>
+  </si>
+  <si>
+    <t>PR6800010-IT-MOT</t>
+  </si>
+  <si>
+    <t>อุปกรณ์+ระบบสแกนใบหน้า</t>
+  </si>
+  <si>
+    <t>office-new</t>
+  </si>
+  <si>
+    <t>IT-6800007</t>
+  </si>
+  <si>
+    <t>IT-6800008</t>
+  </si>
+  <si>
+    <t>IT-6800009</t>
+  </si>
+  <si>
+    <t>PR6800007-IT-MOT</t>
+  </si>
+  <si>
+    <t>PR6800008-IT-MOT</t>
+  </si>
+  <si>
+    <t>PR6800009-IT-MOT</t>
+  </si>
+  <si>
+    <t>Office-new</t>
+  </si>
+  <si>
+    <t>IT-6800011</t>
+  </si>
+  <si>
+    <t>PR6800011-IT-MOT</t>
+  </si>
+  <si>
+    <t>INTERLINK COMMUNICATION PUBLIC COMPANY LIMITED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">อุปกรณ์ Network Office New </t>
+  </si>
+  <si>
+    <t>IT-6800012</t>
+  </si>
+  <si>
+    <t>PR6800012-IT-MOT</t>
+  </si>
+  <si>
+    <t>IP Phone</t>
+  </si>
+  <si>
+    <t>Bing Communications Co,Ltd. (Head office)</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>wifi U6</t>
+  </si>
+  <si>
+    <t>ไพศาล</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>FortiGate 61E Storage SSD 128GB USED, MA Expired</t>
+  </si>
+  <si>
+    <t>IT-6800013</t>
+  </si>
+  <si>
+    <t>PR6800013-IT-MOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">สติ๊กเกอร์ แปะ Smart Pole  งานออกบูธ </t>
+  </si>
+  <si>
+    <t>BKK INKJET</t>
+  </si>
+  <si>
+    <t>IT-6800014</t>
+  </si>
+  <si>
+    <t>PR6800014-IT-MOT</t>
+  </si>
+  <si>
+    <t>รางวายเวย์ 2"x4"</t>
+  </si>
+  <si>
+    <t>IT-6800015</t>
+  </si>
+  <si>
+    <t>PR6800015-IT-MOT</t>
+  </si>
+  <si>
+    <t>V TECH PRO ( THAILAND) CO.,LTD (สำานักงานใหญ่)</t>
+  </si>
+  <si>
+    <t>CAT6 UTP ULTRA w/CROSS FILLER,23AWG,LSZH</t>
+  </si>
+  <si>
+    <t>IT-6800016</t>
+  </si>
+  <si>
+    <t>PR6800016-IT-MOT</t>
+  </si>
+  <si>
+    <t>ระบบกล้อง CCTV</t>
+  </si>
+  <si>
+    <t>IT-6800017</t>
+  </si>
+  <si>
+    <t>PR6800017-IT-MOT</t>
+  </si>
+  <si>
+    <t>TP-LINK AC1300 Mini Wireless MU-MIMO USB Adapter</t>
+  </si>
+  <si>
+    <t>IT-6800018</t>
+  </si>
+  <si>
+    <t>IT-6800019</t>
+  </si>
+  <si>
+    <t>IT-6800020</t>
+  </si>
+  <si>
+    <t>IT-6800021</t>
+  </si>
+  <si>
+    <t>PR6800018-IT-MOT</t>
+  </si>
+  <si>
+    <t>PR6800019-IT-MOT</t>
+  </si>
+  <si>
+    <t>PR6800020-IT-MOT</t>
+  </si>
+  <si>
+    <t>PR6800021-IT-MOT</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkCentre Neo 50t G5</t>
+  </si>
+  <si>
+    <t>Monitor Lenovo L22e-40 (67AFKACBTH)- 3Y.</t>
+  </si>
+  <si>
+    <t>Office Home and Business 2024 Online ESD</t>
+  </si>
+  <si>
+    <t>Office Rayong</t>
+  </si>
+  <si>
+    <t>Rayong</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkPad E14 G6 (Intel)</t>
+  </si>
+  <si>
+    <t>รางวายเวย์ 2x4 ,บล็อค 4x4</t>
+  </si>
+  <si>
+    <t>1.Cable HDTV 4k M/M GLINK / 2.Monitor 24.5 ASUS VG259Q3A</t>
+  </si>
+  <si>
+    <t>IT-6800022</t>
+  </si>
+  <si>
+    <t>PR6800022-IT-MOT</t>
+  </si>
+  <si>
+    <t>1. Unifi U6+ (U6+Plus) Wireless Access Point Wifi6</t>
+  </si>
+  <si>
+    <t>2.injector POE+ 30W Replace U-POE-AT</t>
+  </si>
+  <si>
+    <t>3.Cable PRINTER USB2 (3M TOP TECH)</t>
+  </si>
+  <si>
+    <t>4.UGREEN TYPE-C to 5-in-1 multi-function docking 15596(CM511)</t>
+  </si>
+  <si>
+    <t>LOGITECH M100R MOUSE USB</t>
+  </si>
+  <si>
+    <t>LOGITECH M185 MOUSE WIRELESS MOUSE,2.4GHZ, BLACK</t>
+  </si>
+  <si>
+    <t>IT-6800023</t>
+  </si>
+  <si>
+    <t>PR6800023-IT-MOT</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkBook 14 G7 IML</t>
+  </si>
+  <si>
+    <t>IT-6800024</t>
+  </si>
+  <si>
+    <t>PR6800024-IT-MOT</t>
+  </si>
+  <si>
+    <t>admin sale , Mgr.international</t>
+  </si>
+  <si>
+    <t>IT-6800025</t>
+  </si>
+  <si>
+    <t>PR6800025-IT-MOT</t>
+  </si>
+  <si>
+    <t>Samsung 24" Flat IPS 250cd/㎡, 120Hz, FHD 1920x1080, 5MS, HDMIx2ver1.4</t>
+  </si>
+  <si>
+    <t>IT-6800026</t>
+  </si>
+  <si>
+    <t>PR6800026-IT-MOT</t>
+  </si>
+  <si>
+    <t>พี่จ๊าบ</t>
+  </si>
+  <si>
+    <t>พี่จี๊ด</t>
+  </si>
+  <si>
+    <t>IT-6800027</t>
+  </si>
+  <si>
+    <t>PR6800027-IT-MOT</t>
+  </si>
+  <si>
+    <t>CAT 5E PATCH PANEL 24 PORT ENHANCED</t>
+  </si>
+  <si>
+    <t>Front Mount Shelf Deep 25 CM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INTERLINK COMMUNICATION PUBLIC COMPANY LIMITED</t>
+  </si>
+  <si>
+    <t>IT-6800028</t>
+  </si>
+  <si>
+    <t>PR6800028-IT-MOT</t>
+  </si>
+  <si>
+    <t>SanDisk Ultra microSDXC, SQUAC 256GB, A1, C10, U1, UHS-I,150MB/s R, 4x6, 10Y</t>
+  </si>
+  <si>
+    <t>IT-6800029</t>
+  </si>
+  <si>
+    <t>PR6800029-IT-MOT</t>
+  </si>
+  <si>
+    <t>Microsoft 365 Business Basic</t>
+  </si>
+  <si>
+    <t>CS-200e CARD PRINTER HiTi</t>
+  </si>
+  <si>
+    <t>บริษัท อีซี คอนเนคชั่น จำกัด</t>
+  </si>
+  <si>
+    <t>IT-6800030</t>
+  </si>
+  <si>
+    <t>Epson EcoTank L5590 A3+ Wi-Fi Duplex Wide-Format All-in-One</t>
+  </si>
+  <si>
+    <t>PR6800030-IT-MOT</t>
+  </si>
+  <si>
+    <t>Epson 003 Black  ink bottle</t>
+  </si>
+  <si>
+    <t>Epson 003 Cyan  ink bottle</t>
+  </si>
+  <si>
+    <t>Epson 003 Magenta  ink bottle</t>
+  </si>
+  <si>
+    <t>Epson 003 Yellow  ink bottle</t>
+  </si>
+  <si>
+    <t>IT-6800031</t>
+  </si>
+  <si>
+    <t>PR6800031-IT-MOT</t>
+  </si>
+  <si>
+    <t>Dell 24 Monitor - SE2425H</t>
+  </si>
+  <si>
+    <t>19"GERMAN WALL RACK 12U(60cm.)/B</t>
+  </si>
+  <si>
+    <t>IT-6800032</t>
+  </si>
+  <si>
+    <t>PR6800032-IT-MOT</t>
+  </si>
+  <si>
+    <t>AC Power Distribution 6 TISOutlet w/Cable 3M./B</t>
+  </si>
+  <si>
+    <t>พัดลมระบายอากาศ 4 " ครบชุด</t>
+  </si>
+  <si>
+    <t>LINK CAT 5E PATCH PANEL 24 PORT ENHANCED</t>
+  </si>
+  <si>
+    <t>LINK CABLE MANAGEMENT PANEL 1U with Cover</t>
+  </si>
+  <si>
+    <t>CAT5E LOCKING PLUG BOOT, GREEN (10PCS./PKG) NEW</t>
+  </si>
+  <si>
+    <t>APC EASY UPS BV 800VA/480Watt , AVR, Universal Outlet</t>
+  </si>
+  <si>
+    <t>IT-6800033</t>
+  </si>
+  <si>
+    <t>PR6800033-IT-MOT</t>
+  </si>
+  <si>
+    <t>UniFi U6+ (U6-Plus) อุปกรณ์ Wireless Access Point WiFi6 ความเร็วสูงสุด</t>
+  </si>
+  <si>
+    <t>Catalyst 1200 24-port GE, PoE, 4x1G SFP</t>
+  </si>
+  <si>
+    <t>SNTC-8X5XNBD Catalyst 1200 24-port GE,PoE, 4x1G SFP</t>
+  </si>
+  <si>
+    <t>AC Power cord, 16AWG</t>
+  </si>
+  <si>
+    <t>IT-6800034</t>
+  </si>
+  <si>
+    <t>PR6800034-IT-MOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenovo All In One PC ThinkCentre neo 50a 24 Gen5 </t>
+  </si>
+  <si>
+    <t>IT-6800035</t>
+  </si>
+  <si>
+    <t>PR6800035-IT-MOT</t>
+  </si>
+  <si>
+    <t>Lenovo YogaS7-14 AMD AI7-350 32G 1TB W11 3Y TT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office Home and Business 2024 All Lng APAC EM Retail Online ESD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Win Pro 11 64Bit Eng Intl 1pk DSP OEI DVD</t>
+  </si>
+  <si>
+    <t>IT-6800038</t>
+  </si>
+  <si>
+    <t>PR6800038-IT-MOT</t>
   </si>
 </sst>
 </file>
@@ -146,10 +867,10 @@
     <numFmt numFmtId="166" formatCode="#,###.#"/>
     <numFmt numFmtId="167" formatCode="##"/>
     <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00;\-#,##0.00;;@"/>
-    <numFmt numFmtId="172" formatCode="#,##0;\-#,##0;;@"/>
+    <numFmt numFmtId="169" formatCode="#,##0;\-#,##0;;@"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00;\-#,##0.00;;@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +900,13 @@
       <color theme="1"/>
       <name val="Angsana New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -217,10 +945,34 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Angsana New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -240,6 +992,13 @@
       <color theme="1"/>
       <name val="Angsana New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -302,27 +1061,28 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Angsana New"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Angsana New"/>
-      <family val="1"/>
+      <name val="Angsana News"/>
+      <charset val="222"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Angsana New"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Angsana New"/>
+      <color theme="1"/>
+      <name val="Angsana News"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -352,7 +1112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -681,26 +1441,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="38" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="16" fillId="3" borderId="18" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="37" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="168" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="10" fontId="21" fillId="3" borderId="18" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="37" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="10" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -711,32 +1506,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,15 +1552,15 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -762,62 +1569,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -826,60 +1615,166 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="18" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="18" xfId="29" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -888,98 +1783,115 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="29" xfId="29" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="30" xfId="29" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="23" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="3" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="25" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="25" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="36">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma 2 2" xfId="25" xr:uid="{2C187FC7-A706-48AD-A8C0-D04978BA7C6A}"/>
     <cellStyle name="Comma 2 2 2" xfId="28" xr:uid="{84243DAF-84B1-4EB0-A5D1-55E35697E461}"/>
+    <cellStyle name="Comma 2 2 2 2" xfId="34" xr:uid="{FA91EC6B-8880-4403-9C67-9CE37807E91C}"/>
+    <cellStyle name="Comma 2 2 3" xfId="31" xr:uid="{601445D4-5F2C-49FB-A3C1-18D963614D0F}"/>
     <cellStyle name="Comma 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Comma 3 2" xfId="27" xr:uid="{A374CE4F-F818-4487-A8F0-54C3E275BE81}"/>
+    <cellStyle name="Comma 3 2 2" xfId="33" xr:uid="{F31B32D6-E179-47BA-8860-2153183D4F88}"/>
+    <cellStyle name="Comma 3 3" xfId="30" xr:uid="{19B12952-075D-4AF1-AAD7-C6D0981DB1A8}"/>
     <cellStyle name="Comma 4" xfId="26" xr:uid="{E375430F-066F-4E68-AE7F-12DAE1D32C3B}"/>
     <cellStyle name="Comma 4 2" xfId="29" xr:uid="{41527C7C-6F05-4249-82C1-2BF3BC8F33D3}"/>
+    <cellStyle name="Comma 4 2 2" xfId="35" xr:uid="{A9A02AC1-DFEE-4CBE-942E-EA610FDAF1A8}"/>
+    <cellStyle name="Comma 4 3" xfId="32" xr:uid="{FA52535F-FE25-45EA-8AAE-ACB61FD5FDFF}"/>
     <cellStyle name="comma zerodec" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Currency1" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Dollar (zero dec)" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
@@ -1021,22 +1933,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114483</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>143416</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1407</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>645685</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>173692</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11330</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>33419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A95252C-BE3C-4811-876C-EADDF0D66E16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B63ADCD-3821-90C3-21E5-087D740BC617}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1052,63 +1964,14 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="4515" r="4515"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="114483" y="0"/>
-          <a:ext cx="1034928" cy="764425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>135826</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>197371</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9780</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>6471</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2585934-837D-E188-BE9C-F72C03927A9B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135826" y="763428"/>
-          <a:ext cx="7581040" cy="1333100"/>
+          <a:off x="143416" y="807785"/>
+          <a:ext cx="7566387" cy="1801714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1120,22 +1983,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>533</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>7116</xdr:rowOff>
+      <xdr:colOff>35424</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>94165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>14489</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>32055</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>517026</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>126366</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AD2D1F5-6882-B806-EE3B-AE9A27B09253}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A95252C-BE3C-4811-876C-EADDF0D66E16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1143,22 +2006,15 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect b="56185"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="142047" y="2097173"/>
-          <a:ext cx="7579528" cy="438596"/>
+          <a:off x="180204" y="757105"/>
+          <a:ext cx="866412" cy="606876"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1496,32 +2352,30 @@
   </sheetPr>
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="84" zoomScaleNormal="100" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="54" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="54" customWidth="1"/>
-    <col min="3" max="3" width="33" style="54" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="54" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="58" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="54" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="59" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="54" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="54"/>
-    <col min="10" max="10" width="9.42578125" style="54" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="54"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75">
+    <row r="1" spans="2:10" ht="18">
       <c r="B1" s="5"/>
-      <c r="C1" s="41" t="s">
-        <v>28</v>
+      <c r="C1" s="43" t="s">
+        <v>27</v>
       </c>
       <c r="D1" s="5"/>
-      <c r="E1" s="40"/>
+      <c r="E1" s="42"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -1530,11 +2384,11 @@
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="5"/>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="40"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -1543,84 +2397,99 @@
     </row>
     <row r="3" spans="2:10" ht="13.5" customHeight="1">
       <c r="B3" s="5"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="43" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="17"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="14"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="2:10" ht="17.25" customHeight="1">
       <c r="B4" s="5"/>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="43" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="17"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="5"/>
       <c r="G4" s="84"/>
       <c r="H4" s="84"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="16.5">
+    <row r="5" spans="2:10" s="37" customFormat="1" ht="18.75">
       <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="33" t="s">
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B6" s="52"/>
-      <c r="D6" s="56"/>
-      <c r="F6" s="33" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:10" s="37" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B6" s="50"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="55"/>
+      <c r="F6" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B7" s="49" t="s">
+      <c r="G6" s="18"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" s="37" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B7" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="F7" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="2:10" s="37" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="76"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="B9" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="F7" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="53"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="B9" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="2:10" s="2" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B10" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="92"/>
-      <c r="E10" s="51"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="2:10" ht="18.75">
+      <c r="C9" s="2"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" s="37" customFormat="1" ht="17.25" customHeight="1">
+      <c r="B10" s="92"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="2:10" ht="21">
       <c r="B11" s="85" t="s">
         <v>3</v>
       </c>
@@ -1633,11 +2502,11 @@
         <v>18</v>
       </c>
       <c r="G11" s="86"/>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="28" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="24"/>
+      <c r="J11" s="28"/>
     </row>
     <row r="12" spans="2:10" ht="13.5" customHeight="1">
       <c r="B12" s="87"/>
@@ -1646,7 +2515,7 @@
       <c r="E12" s="90"/>
       <c r="F12" s="91"/>
       <c r="G12" s="86"/>
-      <c r="H12" s="60"/>
+      <c r="H12" s="63"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="2:10" ht="3" customHeight="1" thickBot="1">
@@ -1655,262 +2524,260 @@
       <c r="D13" s="1"/>
       <c r="E13" s="12"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="16"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="66" t="s">
+      <c r="D14" s="107"/>
+      <c r="E14" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="66" t="s">
+      <c r="F14" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="68" t="s">
+      <c r="G14" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="31" t="s">
         <v>9</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1">
-      <c r="B15" s="65"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="39" t="s">
+      <c r="B15" s="101"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="74" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="2:10" ht="21.75" customHeight="1">
-      <c r="B16" s="42"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95">
-        <f>F16*G16</f>
+      <c r="B16" s="44"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="137"/>
+      <c r="H16" s="138">
+        <f>G16*F16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9" ht="21.75" customHeight="1">
       <c r="B17" s="45"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="37"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="46"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="96">
-        <f>F17*G17</f>
+      <c r="F17" s="135"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="140">
+        <f>G17*F17</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B18" s="36"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="48"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="96"/>
       <c r="E18" s="46"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="96">
-        <f t="shared" ref="H18:H32" si="0">F18*G18</f>
+      <c r="F18" s="135"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="140">
+        <f>G18*F18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B19" s="36"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="83"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="82"/>
       <c r="E19" s="46"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="96">
+      <c r="F19" s="135"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="140">
+        <f t="shared" ref="H19:H32" si="0">G19*F19</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B20" s="45"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B20" s="45"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="96">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B21" s="40"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="135"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B21" s="36"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="96">
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B22" s="45"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B22" s="45"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="96">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B23" s="40"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B23" s="36"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="96">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B24" s="40"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B24" s="36"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="96">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B25" s="45"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B25" s="36"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="96">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="135"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B26" s="36"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="96">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B27" s="40"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="135"/>
+      <c r="G27" s="139"/>
+      <c r="H27" s="140">
+        <f>G27*F27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B28" s="40"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B27" s="36"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="96">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B29" s="40"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B28" s="36"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="96">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B30" s="40"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="135"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B29" s="36"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="96">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B31" s="40"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="139"/>
+      <c r="H31" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B30" s="36"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="96">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="2:9" ht="21.75" customHeight="1">
-      <c r="B31" s="36"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="96">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="2:9" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B32" s="25"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="96">
+      <c r="B32" s="29"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="136"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1920,14 +2787,14 @@
       <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="18"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="29"/>
-      <c r="H33" s="103">
+      <c r="G33" s="33"/>
+      <c r="H33" s="141">
         <f>SUM(H16:H32)</f>
         <v>0</v>
       </c>
@@ -1941,25 +2808,25 @@
       <c r="F34" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="30"/>
-      <c r="H34" s="100"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="142"/>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="2:10" ht="22.5" customHeight="1">
       <c r="B35" s="4"/>
-      <c r="C35" s="34"/>
+      <c r="C35" s="39"/>
       <c r="D35" s="1"/>
       <c r="E35" s="12"/>
       <c r="F35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="30"/>
-      <c r="H35" s="104">
+      <c r="G35" s="34"/>
+      <c r="H35" s="143">
         <f>H33-H34</f>
         <v>0</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="57"/>
+      <c r="J35" s="32"/>
     </row>
     <row r="36" spans="2:10" ht="22.5" customHeight="1" thickBot="1">
       <c r="B36" s="4"/>
@@ -1969,532 +2836,518 @@
       <c r="F36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="31"/>
-      <c r="H36" s="105">
+      <c r="G36" s="35"/>
+      <c r="H36" s="144">
         <f>H35*7%</f>
         <v>0</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1">
-      <c r="B37" s="74" t="str">
-        <f>BAHTTEXT(H37)</f>
-        <v>ศูนย์บาทถ้วน</v>
-      </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="76"/>
+      <c r="B37" s="110"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="112"/>
       <c r="F37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="32"/>
-      <c r="H37" s="106">
-        <f>H35+H36</f>
+      <c r="G37" s="36"/>
+      <c r="H37" s="145">
+        <f>SUM(H35:H36)</f>
         <v>0</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="2:10" ht="27.75" customHeight="1">
       <c r="B38" s="3"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="6"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B39" s="81" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="77"/>
+      <c r="B39" s="117" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="113"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="12"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="78"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="114"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="2:10" ht="19.5" customHeight="1">
-      <c r="B40" s="81"/>
-      <c r="C40" s="77"/>
+      <c r="B40" s="117"/>
+      <c r="C40" s="113"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="78"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113"/>
+      <c r="G40" s="113"/>
+      <c r="H40" s="114"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B41" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="23" t="s">
+      <c r="B41" s="115" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="116"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="63"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="98"/>
+      <c r="H41" s="99"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="18.75">
+    <row r="42" spans="2:10" ht="21">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="12"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
+      <c r="G42" s="97"/>
+      <c r="H42" s="97"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:10" ht="18.75">
+    <row r="43" spans="2:10" ht="21">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="12"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="16"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:10" ht="18.75">
+    <row r="44" spans="2:10" ht="21">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="12"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="16"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:10" ht="18.75">
+    <row r="45" spans="2:10" ht="21">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="12"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="16"/>
+      <c r="G45" s="20"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:10" ht="18.75">
+    <row r="46" spans="2:10" ht="21">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="12"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="16"/>
+      <c r="G46" s="20"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:10" ht="18.75">
+    <row r="47" spans="2:10" ht="21">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="12"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="16"/>
+      <c r="G47" s="20"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="2:10" ht="18.75">
+    <row r="48" spans="2:10" ht="21">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="12"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="16"/>
+      <c r="G48" s="20"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" ht="18.75">
+    <row r="49" spans="2:9" ht="21">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="12"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="16"/>
+      <c r="G49" s="20"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" ht="18.75">
+    <row r="50" spans="2:9" ht="21">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="12"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="16"/>
+      <c r="G50" s="20"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="2:9" ht="18.75">
+    <row r="51" spans="2:9" ht="21">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="12"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="16"/>
+      <c r="G51" s="20"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" ht="18.75">
+    <row r="52" spans="2:9" ht="21">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="12"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="16"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:9" ht="18.75">
+    <row r="53" spans="2:9" ht="21">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="12"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="16"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="2:9" ht="18.75">
+    <row r="54" spans="2:9" ht="21">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="12"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="16"/>
+      <c r="G54" s="20"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="2:9" ht="18.75">
+    <row r="55" spans="2:9" ht="21">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="12"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="16"/>
+      <c r="G55" s="20"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="2:9" ht="18.75">
+    <row r="56" spans="2:9" ht="21">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="12"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="16"/>
+      <c r="G56" s="20"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="2:9" ht="18.75">
+    <row r="57" spans="2:9" ht="21">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="12"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="16"/>
+      <c r="G57" s="20"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="2:9" ht="18.75">
+    <row r="58" spans="2:9" ht="21">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="12"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="16"/>
+      <c r="G58" s="20"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="2:9" ht="18.75">
+    <row r="59" spans="2:9" ht="21">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="12"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="16"/>
+      <c r="G59" s="20"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="2:9" ht="18.75">
+    <row r="60" spans="2:9" ht="21">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="12"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="16"/>
+      <c r="G60" s="20"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="2:9" ht="18.75">
+    <row r="61" spans="2:9" ht="21">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="12"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="16"/>
+      <c r="G61" s="20"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="2:9" ht="18.75">
+    <row r="62" spans="2:9" ht="21">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="12"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="16"/>
+      <c r="G62" s="20"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="2:9" ht="18.75">
+    <row r="63" spans="2:9" ht="21">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="12"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="16"/>
+      <c r="G63" s="20"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="2:9" ht="18.75">
+    <row r="64" spans="2:9" ht="21">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="12"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="16"/>
+      <c r="G64" s="20"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:9" ht="18.75">
+    <row r="65" spans="2:9" ht="21">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="12"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="16"/>
+      <c r="G65" s="20"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="2:9" ht="18.75">
+    <row r="66" spans="2:9" ht="21">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="12"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="16"/>
+      <c r="G66" s="20"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="2:9" ht="18.75">
+    <row r="67" spans="2:9" ht="21">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="12"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="16"/>
+      <c r="G67" s="20"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="2:9" ht="18.75">
+    <row r="68" spans="2:9" ht="21">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="12"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="16"/>
+      <c r="G68" s="20"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="2:9" ht="18.75">
+    <row r="69" spans="2:9" ht="21">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="12"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="16"/>
+      <c r="G69" s="20"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" ht="18.75">
+    <row r="70" spans="2:9" ht="21">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="12"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="16"/>
+      <c r="G70" s="20"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" ht="18.75">
+    <row r="71" spans="2:9" ht="21">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="12"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="16"/>
+      <c r="G71" s="20"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:9" ht="18.75">
+    <row r="72" spans="2:9" ht="21">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="12"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="16"/>
+      <c r="G72" s="20"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="2:9" ht="18.75">
+    <row r="73" spans="2:9" ht="21">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="12"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="16"/>
+      <c r="G73" s="20"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="2:9" ht="18.75">
+    <row r="74" spans="2:9" ht="21">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="12"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="16"/>
+      <c r="G74" s="20"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="2:9" ht="18.75">
+    <row r="75" spans="2:9" ht="21">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="12"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="16"/>
+      <c r="G75" s="20"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:9" ht="18.75">
+    <row r="76" spans="2:9" ht="21">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="12"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="16"/>
+      <c r="G76" s="20"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="2:9" ht="18.75">
+    <row r="77" spans="2:9" ht="21">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="12"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="16"/>
+      <c r="G77" s="20"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="2:9" ht="18.75">
+    <row r="78" spans="2:9" ht="21">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="12"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="16"/>
+      <c r="G78" s="20"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="2:9" ht="18.75">
+    <row r="79" spans="2:9" ht="21">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="12"/>
       <c r="F79" s="1"/>
-      <c r="G79" s="16"/>
+      <c r="G79" s="20"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="2:9" ht="18.75">
+    <row r="80" spans="2:9" ht="21">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="12"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="16"/>
+      <c r="G80" s="20"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="2:9" ht="18.75">
+    <row r="81" spans="2:9" ht="21">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="12"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="16"/>
+      <c r="G81" s="20"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="2:9" ht="18.75">
+    <row r="82" spans="2:9" ht="21">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="12"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="16"/>
+      <c r="G82" s="20"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="2:9" ht="18.75">
+    <row r="83" spans="2:9" ht="21">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="12"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="16"/>
+      <c r="G83" s="20"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="2:9" ht="18.75">
+    <row r="84" spans="2:9" ht="21">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="12"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="16"/>
+      <c r="G84" s="20"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="2:9" ht="18.75">
+    <row r="85" spans="2:9" ht="21">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="12"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="16"/>
+      <c r="G85" s="20"/>
       <c r="H85" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="C7:D7"/>
+  <mergeCells count="30">
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B14:B15"/>
@@ -2511,11 +3364,1600 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="27" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="87" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="89" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E2E9DB-DC53-49CA-83CB-C137D0B49FB3}">
+  <dimension ref="A1:F95"/>
+  <sheetViews>
+    <sheetView topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="75" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="75" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21">
+      <c r="A2" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21">
+      <c r="A3" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21">
+      <c r="A4" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21">
+      <c r="A5" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21">
+      <c r="A6" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A7" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="129" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="121" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="131" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="130"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="21">
+      <c r="A10" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21">
+      <c r="A11" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="21">
+      <c r="A12" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="21">
+      <c r="A13" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21">
+      <c r="A14" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.45" customHeight="1">
+      <c r="A15" s="124" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="126" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="126" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="133" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="123" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.45" customHeight="1">
+      <c r="A16" s="125"/>
+      <c r="B16" s="127"/>
+      <c r="C16" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="127"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="123"/>
+    </row>
+    <row r="17" spans="1:6" ht="21">
+      <c r="A17" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="21">
+      <c r="A18" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="21">
+      <c r="A19" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18.75">
+      <c r="A20" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="21">
+      <c r="A21" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="21">
+      <c r="A22" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="21">
+      <c r="A23" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="121" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="128" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="21">
+      <c r="A24" s="120"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="128"/>
+    </row>
+    <row r="25" spans="1:6" ht="21">
+      <c r="A25" s="119" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="121" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="121" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="21">
+      <c r="A26" s="120"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+    </row>
+    <row r="27" spans="1:6" ht="21">
+      <c r="A27" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="21">
+      <c r="A28" s="119" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="121" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="121" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="21">
+      <c r="A29" s="120"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="122"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
+    </row>
+    <row r="30" spans="1:6" ht="21">
+      <c r="A30" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="21">
+      <c r="A31" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="21">
+      <c r="A32" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="79" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="21">
+      <c r="A33" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="75" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="21">
+      <c r="A34" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="21">
+      <c r="A35" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="75" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="F36" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="21">
+      <c r="A37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="F37" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="21">
+      <c r="A38" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="61" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="F38" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="21">
+      <c r="A39" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="F40" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="21">
+      <c r="A41" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="21">
+      <c r="A42" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="21">
+      <c r="A43" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="E43" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="21">
+      <c r="A44" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="21">
+      <c r="A45" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="21">
+      <c r="A46" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D46" s="75" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="21">
+      <c r="A47" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" s="75" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="21">
+      <c r="A48" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" s="118" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="118" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="118" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="118"/>
+      <c r="B49" s="118"/>
+      <c r="C49" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="D49" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+    </row>
+    <row r="50" spans="1:6" ht="21">
+      <c r="A50" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="118" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="118" t="s">
+        <v>199</v>
+      </c>
+      <c r="F50" s="118" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="21">
+      <c r="A51" s="118"/>
+      <c r="B51" s="118"/>
+      <c r="C51" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D51" s="118"/>
+      <c r="E51" s="118"/>
+      <c r="F51" s="118"/>
+    </row>
+    <row r="52" spans="1:6" ht="21">
+      <c r="A52" s="118"/>
+      <c r="B52" s="118"/>
+      <c r="C52" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" s="118"/>
+      <c r="E52" s="118"/>
+      <c r="F52" s="118"/>
+    </row>
+    <row r="53" spans="1:6" ht="21">
+      <c r="A53" s="118"/>
+      <c r="B53" s="118"/>
+      <c r="C53" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="118"/>
+      <c r="E53" s="118"/>
+      <c r="F53" s="118"/>
+    </row>
+    <row r="54" spans="1:6" ht="21">
+      <c r="A54" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C54" s="77" t="s">
+        <v>203</v>
+      </c>
+      <c r="D54" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="75" t="s">
+        <v>199</v>
+      </c>
+      <c r="F54" s="75" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C56" t="s">
+        <v>206</v>
+      </c>
+      <c r="D56" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="118" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="118" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="C57" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" s="118"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="118"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="C58" t="s">
+        <v>208</v>
+      </c>
+      <c r="D58" s="118"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="118"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="C59" t="s">
+        <v>209</v>
+      </c>
+      <c r="D59" s="118"/>
+      <c r="E59" s="118"/>
+      <c r="F59" s="118"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" t="s">
+        <v>210</v>
+      </c>
+      <c r="D60" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F60" s="118" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="C61" t="s">
+        <v>211</v>
+      </c>
+      <c r="D61" s="118"/>
+      <c r="E61" s="118"/>
+      <c r="F61" s="118"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C62" t="s">
+        <v>214</v>
+      </c>
+      <c r="D62" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" s="118" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="C63" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63" s="118"/>
+      <c r="E63" s="118"/>
+      <c r="F63" s="118"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C64" t="s">
+        <v>220</v>
+      </c>
+      <c r="D64" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" s="75" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" t="s">
+        <v>214</v>
+      </c>
+      <c r="D65" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65" s="118" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="C66" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66" s="118"/>
+      <c r="E66" s="118"/>
+      <c r="F66" s="118"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C67" t="s">
+        <v>227</v>
+      </c>
+      <c r="D67" s="118" t="s">
+        <v>229</v>
+      </c>
+      <c r="E67" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67" s="118" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="C68" t="s">
+        <v>181</v>
+      </c>
+      <c r="D68" s="118"/>
+      <c r="E68" s="118"/>
+      <c r="F68" s="118"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="C69" t="s">
+        <v>228</v>
+      </c>
+      <c r="D69" s="118"/>
+      <c r="E69" s="118"/>
+      <c r="F69" s="118"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C70" t="s">
+        <v>235</v>
+      </c>
+      <c r="D70" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="75" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="75" t="s">
+        <v>237</v>
+      </c>
+      <c r="E71" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F71" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C72" t="s">
+        <v>239</v>
+      </c>
+      <c r="D72" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72" s="118" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="C73" t="s">
+        <v>241</v>
+      </c>
+      <c r="D73" s="118"/>
+      <c r="E73" s="118"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="C74" t="s">
+        <v>242</v>
+      </c>
+      <c r="D74" s="118"/>
+      <c r="E74" s="118"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="C75" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="D75" s="118"/>
+      <c r="E75" s="118"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="C76" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" s="118"/>
+      <c r="E76" s="118"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="75" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C78" t="s">
+        <v>248</v>
+      </c>
+      <c r="D78" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E78" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F78" s="118" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="C79" t="s">
+        <v>251</v>
+      </c>
+      <c r="D79" s="118"/>
+      <c r="E79" s="118"/>
+      <c r="F79" s="118"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="C80" t="s">
+        <v>252</v>
+      </c>
+      <c r="D80" s="118"/>
+      <c r="E80" s="118"/>
+      <c r="F80" s="118"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="C81" s="80" t="s">
+        <v>253</v>
+      </c>
+      <c r="D81" s="118"/>
+      <c r="E81" s="118"/>
+      <c r="F81" s="118"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="C82" s="80" t="s">
+        <v>254</v>
+      </c>
+      <c r="D82" s="118"/>
+      <c r="E82" s="118"/>
+      <c r="F82" s="118"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="C83" s="80" t="s">
+        <v>255</v>
+      </c>
+      <c r="D83" s="118"/>
+      <c r="E83" s="118"/>
+      <c r="F83" s="118"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C84" t="s">
+        <v>256</v>
+      </c>
+      <c r="D84" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F84" s="118" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="C85" t="s">
+        <v>259</v>
+      </c>
+      <c r="D85" s="118"/>
+      <c r="E85" s="118"/>
+      <c r="F85" s="118"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="C86" t="s">
+        <v>260</v>
+      </c>
+      <c r="D86" s="118"/>
+      <c r="E86" s="118"/>
+      <c r="F86" s="118"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="C87" s="80" t="s">
+        <v>261</v>
+      </c>
+      <c r="D87" s="118"/>
+      <c r="E87" s="118"/>
+      <c r="F87" s="118"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="C88" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="D88" s="118"/>
+      <c r="E88" s="118"/>
+      <c r="F88" s="118"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C89" t="s">
+        <v>265</v>
+      </c>
+      <c r="D89" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E89" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F89" s="118" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="C90" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="118"/>
+      <c r="E90" s="118"/>
+      <c r="F90" s="118"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C91" t="s">
+        <v>232</v>
+      </c>
+      <c r="D91" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E91" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F91" s="75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E93" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="F93" s="118" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="C94" t="s">
+        <v>269</v>
+      </c>
+      <c r="D94" s="118"/>
+      <c r="E94" s="118"/>
+      <c r="F94" s="118"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="C95" t="s">
+        <v>270</v>
+      </c>
+      <c r="D95" s="118"/>
+      <c r="E95" s="118"/>
+      <c r="F95" s="118"/>
+    </row>
+  </sheetData>
+  <mergeCells count="62">
+    <mergeCell ref="F78:F83"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="F84:F88"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="D78:D83"/>
+    <mergeCell ref="E78:E83"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="E72:E76"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="E67:E69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="D93:D95"/>
+    <mergeCell ref="E93:E95"/>
+    <mergeCell ref="F93:F95"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="F56:F59"/>
+    <mergeCell ref="D72:D76"/>
+  </mergeCells>
+  <phoneticPr fontId="27" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check 0 for index
</commit_message>
<xml_diff>
--- a/public/templates/PO_Form.xlsx
+++ b/public/templates/PO_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\motassetlistit\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB778617-3D85-48CE-8804-A6996D90BF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE82FE40-DF81-44E5-AE3C-FBE7EC544F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -911,6 +911,63 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -957,63 +1014,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="36">
@@ -1372,15 +1372,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1038</xdr:colOff>
+      <xdr:colOff>3419</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>18015</xdr:rowOff>
+      <xdr:rowOff>15633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>153248</xdr:colOff>
+      <xdr:colOff>156770</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>30092</xdr:rowOff>
+      <xdr:rowOff>31083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1409,8 +1409,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="143913" y="2113515"/>
-          <a:ext cx="152210" cy="421652"/>
+          <a:off x="146294" y="2139708"/>
+          <a:ext cx="153351" cy="453600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1422,15 +1422,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>763264</xdr:colOff>
+      <xdr:colOff>765644</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>15631</xdr:rowOff>
+      <xdr:rowOff>16669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1919</xdr:colOff>
+      <xdr:colOff>4196</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>27708</xdr:rowOff>
+      <xdr:rowOff>32119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1459,8 +1459,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7564114" y="2111131"/>
-          <a:ext cx="134005" cy="421652"/>
+          <a:off x="7566494" y="2140744"/>
+          <a:ext cx="133902" cy="453600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1848,8 +1848,8 @@
   </sheetPr>
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="E4" zoomScale="340" zoomScaleNormal="100" zoomScaleSheetLayoutView="340" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1865,7 +1865,7 @@
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75">
+    <row r="1" spans="2:10" ht="18">
       <c r="B1" s="5"/>
       <c r="C1" s="43" t="s">
         <v>27</v>
@@ -1912,16 +1912,16 @@
       <c r="D4" s="5"/>
       <c r="E4" s="21"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="2:10" s="37" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B5" s="88"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="38" t="s">
         <v>16</v>
       </c>
@@ -1944,8 +1944,8 @@
       <c r="B7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
       <c r="F7" s="38" t="s">
         <v>1</v>
       </c>
@@ -1976,8 +1976,8 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:10" s="37" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="112"/>
       <c r="D10" s="2"/>
       <c r="E10" s="49"/>
       <c r="F10" s="2"/>
@@ -1985,19 +1985,19 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:10" ht="18.75">
-      <c r="B11" s="81" t="s">
+    <row r="11" spans="2:10" ht="21">
+      <c r="B11" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="84" t="s">
+      <c r="C11" s="103"/>
+      <c r="D11" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="82"/>
-      <c r="F11" s="84" t="s">
+      <c r="E11" s="103"/>
+      <c r="F11" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="82"/>
+      <c r="G11" s="103"/>
       <c r="H11" s="28" t="s">
         <v>21</v>
       </c>
@@ -2005,12 +2005,12 @@
       <c r="J11" s="28"/>
     </row>
     <row r="12" spans="2:10" ht="13.5" customHeight="1">
-      <c r="B12" s="83"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="82"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="103"/>
       <c r="H12" s="52"/>
       <c r="I12" s="1"/>
     </row>
@@ -2025,20 +2025,20 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="2:10" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="100" t="s">
+      <c r="D14" s="88"/>
+      <c r="E14" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="100" t="s">
+      <c r="F14" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="102" t="s">
+      <c r="G14" s="85" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="31" t="s">
@@ -2047,12 +2047,12 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="12" customHeight="1" thickBot="1">
-      <c r="B15" s="99"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="103"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="86"/>
       <c r="H15" s="63" t="s">
         <v>17</v>
       </c>
@@ -2086,8 +2086,8 @@
     </row>
     <row r="18" spans="2:9" ht="21.75" customHeight="1">
       <c r="B18" s="45"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="93"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="114"/>
       <c r="E18" s="46"/>
       <c r="F18" s="65"/>
       <c r="G18" s="69"/>
@@ -2099,8 +2099,8 @@
     </row>
     <row r="19" spans="2:9" ht="21.75" customHeight="1">
       <c r="B19" s="40"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="99"/>
       <c r="E19" s="46"/>
       <c r="F19" s="65"/>
       <c r="G19" s="69"/>
@@ -2151,8 +2151,8 @@
     </row>
     <row r="23" spans="2:9" ht="21.75" customHeight="1">
       <c r="B23" s="40"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="99"/>
       <c r="E23" s="46"/>
       <c r="F23" s="65"/>
       <c r="G23" s="69"/>
@@ -2164,8 +2164,8 @@
     </row>
     <row r="24" spans="2:9" ht="21.75" customHeight="1">
       <c r="B24" s="40"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="99"/>
       <c r="E24" s="46"/>
       <c r="F24" s="65"/>
       <c r="G24" s="69"/>
@@ -2216,8 +2216,8 @@
     </row>
     <row r="28" spans="2:9" ht="21.75" customHeight="1">
       <c r="B28" s="40"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="78"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="99"/>
       <c r="E28" s="46"/>
       <c r="F28" s="65"/>
       <c r="G28" s="69"/>
@@ -2229,8 +2229,8 @@
     </row>
     <row r="29" spans="2:9" ht="21.75" customHeight="1">
       <c r="B29" s="40"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="78"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="99"/>
       <c r="E29" s="46"/>
       <c r="F29" s="65"/>
       <c r="G29" s="69"/>
@@ -2340,10 +2340,10 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="2:10" ht="23.25" customHeight="1" thickBot="1">
-      <c r="B37" s="108"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="110"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="92"/>
+      <c r="D37" s="92"/>
+      <c r="E37" s="93"/>
       <c r="F37" s="11" t="s">
         <v>13</v>
       </c>
@@ -2365,54 +2365,54 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="2:10" ht="34.5" customHeight="1">
-      <c r="B39" s="114" t="s">
+      <c r="B39" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="94"/>
+      <c r="C39" s="77"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="12"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="111"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="94"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="2:10" ht="19.5" customHeight="1">
-      <c r="B40" s="114"/>
-      <c r="C40" s="94"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="77"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="94"/>
-      <c r="G40" s="94"/>
-      <c r="H40" s="111"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="94"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="2:10" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B41" s="112" t="s">
+      <c r="B41" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="113"/>
+      <c r="C41" s="96"/>
       <c r="D41" s="24"/>
       <c r="E41" s="27" t="s">
         <v>20</v>
       </c>
       <c r="F41" s="27"/>
-      <c r="G41" s="96"/>
-      <c r="H41" s="97"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="80"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:10" ht="18.75">
+    <row r="42" spans="2:10" ht="21">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="12"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:10" ht="18.75">
+    <row r="43" spans="2:10" ht="21">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2422,7 +2422,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:10" ht="18.75">
+    <row r="44" spans="2:10" ht="21">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2432,7 +2432,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:10" ht="18.75">
+    <row r="45" spans="2:10" ht="21">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2442,7 +2442,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:10" ht="18.75">
+    <row r="46" spans="2:10" ht="21">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2452,7 +2452,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:10" ht="18.75">
+    <row r="47" spans="2:10" ht="21">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2462,7 +2462,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="2:10" ht="18.75">
+    <row r="48" spans="2:10" ht="21">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2472,7 +2472,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" ht="18.75">
+    <row r="49" spans="2:9" ht="21">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2482,7 +2482,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" ht="18.75">
+    <row r="50" spans="2:9" ht="21">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2492,7 +2492,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="2:9" ht="18.75">
+    <row r="51" spans="2:9" ht="21">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2502,7 +2502,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" ht="18.75">
+    <row r="52" spans="2:9" ht="21">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2512,7 +2512,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:9" ht="18.75">
+    <row r="53" spans="2:9" ht="21">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2522,7 +2522,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="2:9" ht="18.75">
+    <row r="54" spans="2:9" ht="21">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2532,7 +2532,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="2:9" ht="18.75">
+    <row r="55" spans="2:9" ht="21">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2542,7 +2542,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="2:9" ht="18.75">
+    <row r="56" spans="2:9" ht="21">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2552,7 +2552,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="2:9" ht="18.75">
+    <row r="57" spans="2:9" ht="21">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2562,7 +2562,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="2:9" ht="18.75">
+    <row r="58" spans="2:9" ht="21">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2572,7 +2572,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="2:9" ht="18.75">
+    <row r="59" spans="2:9" ht="21">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2582,7 +2582,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="2:9" ht="18.75">
+    <row r="60" spans="2:9" ht="21">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2592,7 +2592,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="2:9" ht="18.75">
+    <row r="61" spans="2:9" ht="21">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2602,7 +2602,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="2:9" ht="18.75">
+    <row r="62" spans="2:9" ht="21">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2612,7 +2612,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="2:9" ht="18.75">
+    <row r="63" spans="2:9" ht="21">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2622,7 +2622,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="2:9" ht="18.75">
+    <row r="64" spans="2:9" ht="21">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2632,7 +2632,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:9" ht="18.75">
+    <row r="65" spans="2:9" ht="21">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2642,7 +2642,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="2:9" ht="18.75">
+    <row r="66" spans="2:9" ht="21">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2652,7 +2652,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="2:9" ht="18.75">
+    <row r="67" spans="2:9" ht="21">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2662,7 +2662,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="2:9" ht="18.75">
+    <row r="68" spans="2:9" ht="21">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2672,7 +2672,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="2:9" ht="18.75">
+    <row r="69" spans="2:9" ht="21">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2682,7 +2682,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="2:9" ht="18.75">
+    <row r="70" spans="2:9" ht="21">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2692,7 +2692,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="2:9" ht="18.75">
+    <row r="71" spans="2:9" ht="21">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2702,7 +2702,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:9" ht="18.75">
+    <row r="72" spans="2:9" ht="21">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2712,7 +2712,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="2:9" ht="18.75">
+    <row r="73" spans="2:9" ht="21">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2722,7 +2722,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="2:9" ht="18.75">
+    <row r="74" spans="2:9" ht="21">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2732,7 +2732,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="2:9" ht="18.75">
+    <row r="75" spans="2:9" ht="21">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2742,7 +2742,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:9" ht="18.75">
+    <row r="76" spans="2:9" ht="21">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2752,7 +2752,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="2:9" ht="18.75">
+    <row r="77" spans="2:9" ht="21">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2762,7 +2762,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="2:9" ht="18.75">
+    <row r="78" spans="2:9" ht="21">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2772,7 +2772,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="2:9" ht="18.75">
+    <row r="79" spans="2:9" ht="21">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2782,7 +2782,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="2:9" ht="18.75">
+    <row r="80" spans="2:9" ht="21">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2792,7 +2792,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="2:9" ht="18.75">
+    <row r="81" spans="2:9" ht="21">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2802,7 +2802,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="2:9" ht="18.75">
+    <row r="82" spans="2:9" ht="21">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2812,7 +2812,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="2:9" ht="18.75">
+    <row r="83" spans="2:9" ht="21">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2822,7 +2822,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="2:9" ht="18.75">
+    <row r="84" spans="2:9" ht="21">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2832,7 +2832,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="2:9" ht="18.75">
+    <row r="85" spans="2:9" ht="21">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2843,6 +2843,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G41:H41"/>
@@ -2859,20 +2873,6 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>